<commit_message>
integrating the part2 data and starting the analysis
</commit_message>
<xml_diff>
--- a/data/exp_pro/integration_results.xlsx
+++ b/data/exp_pro/integration_results.xlsx
@@ -30,7 +30,7 @@
     <t>sample</t>
   </si>
   <si>
-    <t>k_no3</t>
+    <t>r_no3</t>
   </si>
   <si>
     <t>c₀</t>
@@ -560,7 +560,7 @@
         <v>0.0028888213005892906</v>
       </c>
       <c r="D2">
-        <v>0.9837702690124213</v>
+        <v>0.9837702690124214</v>
       </c>
       <c r="E2">
         <v>0.0</v>
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>7.118242216056418e-6</v>
+        <v>7.118242216056422e-6</v>
       </c>
       <c r="C3">
         <v>0.0023564174254191994</v>
@@ -624,13 +624,13 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3.578991348692013e-6</v>
+        <v>3.578991348692008e-6</v>
       </c>
       <c r="C4">
-        <v>0.0030066570304212066</v>
+        <v>0.0030066570304212057</v>
       </c>
       <c r="D4">
-        <v>0.8537160291503736</v>
+        <v>0.8537160291503734</v>
       </c>
       <c r="E4">
         <v>0.0</v>
@@ -659,13 +659,13 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>4.256655561104177e-6</v>
+        <v>4.256655561104181e-6</v>
       </c>
       <c r="C5">
         <v>0.0030570173834040654</v>
       </c>
       <c r="D5">
-        <v>0.9133514435885821</v>
+        <v>0.9133514435885822</v>
       </c>
       <c r="E5">
         <v>0.0</v>
@@ -694,25 +694,25 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>3.478385067915703e-6</v>
+        <v>3.4783850679157055e-6</v>
       </c>
       <c r="C6">
-        <v>0.001878330822536063</v>
+        <v>0.0018783308225360635</v>
       </c>
       <c r="D6">
-        <v>0.8896796967247943</v>
+        <v>0.8896796967247942</v>
       </c>
       <c r="E6">
         <v>65.0</v>
       </c>
       <c r="F6">
-        <v>0.03066537200626146</v>
+        <v>0.030665372006261377</v>
       </c>
       <c r="G6">
-        <v>0.0011328828073544777</v>
+        <v>0.0011328828073544773</v>
       </c>
       <c r="H6">
-        <v>27.068441507971706</v>
+        <v>27.06844150797164</v>
       </c>
       <c r="I6">
         <v>3.0</v>
@@ -729,13 +729,13 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>4.091694782436054e-6</v>
+        <v>4.091694782436062e-6</v>
       </c>
       <c r="C7">
-        <v>0.0016430538673954224</v>
+        <v>0.0016430538673954237</v>
       </c>
       <c r="D7">
-        <v>0.932307420901188</v>
+        <v>0.9323074209011878</v>
       </c>
       <c r="E7">
         <v>65.0</v>
@@ -744,10 +744,10 @@
         <v>0.05978778447761897</v>
       </c>
       <c r="G7">
-        <v>0.001344935791486376</v>
+        <v>0.0013449357914863747</v>
       </c>
       <c r="H7">
-        <v>44.454006545207335</v>
+        <v>44.45400654520738</v>
       </c>
       <c r="I7">
         <v>5.56500000000003</v>
@@ -764,10 +764,10 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>2.9827722191945188e-6</v>
+        <v>2.982772219194521e-6</v>
       </c>
       <c r="C8">
-        <v>0.0005430912093717703</v>
+        <v>0.0005430912093717706</v>
       </c>
       <c r="D8">
         <v>0.8949963838513406</v>
@@ -776,13 +776,13 @@
         <v>10.0</v>
       </c>
       <c r="F8">
-        <v>0.003449922016771724</v>
+        <v>0.0034499220167717136</v>
       </c>
       <c r="G8">
-        <v>0.0006453632514853554</v>
+        <v>0.0006453632514853551</v>
       </c>
       <c r="H8">
-        <v>5.3457057073383885</v>
+        <v>5.345705707338374</v>
       </c>
       <c r="I8">
         <v>17.325</v>
@@ -799,22 +799,22 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <v>5.019661997769568e-6</v>
+        <v>5.0196619977695655e-6</v>
       </c>
       <c r="C9">
-        <v>0.0006868574715319702</v>
+        <v>0.0006868574715319699</v>
       </c>
       <c r="D9">
-        <v>0.720798913670701</v>
+        <v>0.7207989136707009</v>
       </c>
       <c r="E9">
         <v>20.0</v>
       </c>
       <c r="F9">
-        <v>0.021942804736290688</v>
+        <v>0.02194280473629069</v>
       </c>
       <c r="G9">
-        <v>0.002537887669577846</v>
+        <v>0.0025378876695778462</v>
       </c>
       <c r="H9">
         <v>8.646089816867534</v>
@@ -834,25 +834,25 @@
         <v>26</v>
       </c>
       <c r="B10">
-        <v>1.797695820229706e-6</v>
+        <v>1.797695820229746e-6</v>
       </c>
       <c r="C10">
-        <v>0.002217974601471786</v>
+        <v>0.002217974601471791</v>
       </c>
       <c r="D10">
-        <v>0.5815823553007151</v>
+        <v>0.5815823553007161</v>
       </c>
       <c r="E10">
         <v>50.0</v>
       </c>
       <c r="F10">
-        <v>0.023330941880924133</v>
+        <v>0.02333094188092394</v>
       </c>
       <c r="G10">
-        <v>0.0009650802861258072</v>
+        <v>0.0009650802861258024</v>
       </c>
       <c r="H10">
-        <v>24.175130521610022</v>
+        <v>24.17513052160994</v>
       </c>
       <c r="I10">
         <v>13.135</v>
@@ -869,13 +869,13 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <v>2.8192432208924366e-6</v>
+        <v>2.8192432208924357e-6</v>
       </c>
       <c r="C11">
         <v>0.0009498658740996753</v>
       </c>
       <c r="D11">
-        <v>0.9333396189006049</v>
+        <v>0.933339618900605</v>
       </c>
       <c r="E11">
         <v>30.0</v>
@@ -904,13 +904,13 @@
         <v>28</v>
       </c>
       <c r="B12">
-        <v>2.6781060098100353e-6</v>
+        <v>2.67810600981003e-6</v>
       </c>
       <c r="C12">
-        <v>0.0024028065253989344</v>
+        <v>0.002402806525398934</v>
       </c>
       <c r="D12">
-        <v>0.732642805778622</v>
+        <v>0.7326428057786221</v>
       </c>
       <c r="E12">
         <v>0.0</v>
@@ -939,13 +939,13 @@
         <v>29</v>
       </c>
       <c r="B13">
-        <v>4.48994384879435e-6</v>
+        <v>4.4899438487943405e-6</v>
       </c>
       <c r="C13">
-        <v>0.003049855920034846</v>
+        <v>0.0030498559200348454</v>
       </c>
       <c r="D13">
-        <v>0.7790251813239407</v>
+        <v>0.7790251813239406</v>
       </c>
       <c r="E13">
         <v>0.0</v>
@@ -980,7 +980,7 @@
         <v>0.002235039336088827</v>
       </c>
       <c r="D14">
-        <v>0.8725628538092223</v>
+        <v>0.8725628538092224</v>
       </c>
       <c r="E14">
         <v>30.0</v>
@@ -1009,25 +1009,25 @@
         <v>32</v>
       </c>
       <c r="B15">
-        <v>4.277303779273057e-6</v>
+        <v>4.277303779273037e-6</v>
       </c>
       <c r="C15">
-        <v>0.0023812930023717253</v>
+        <v>0.0023812930023717226</v>
       </c>
       <c r="D15">
-        <v>0.7424761480330688</v>
+        <v>0.7424761480330686</v>
       </c>
       <c r="E15">
         <v>65.0</v>
       </c>
       <c r="F15">
-        <v>0.032596417897305746</v>
+        <v>0.03259641789730591</v>
       </c>
       <c r="G15">
-        <v>0.0007214456521539652</v>
+        <v>0.0007214456521539678</v>
       </c>
       <c r="H15">
-        <v>45.18208377857031</v>
+        <v>45.18208377857037</v>
       </c>
       <c r="I15">
         <v>3.55500000000002</v>
@@ -1044,13 +1044,13 @@
         <v>33</v>
       </c>
       <c r="B16">
-        <v>3.7545351797626435e-6</v>
+        <v>3.754535179762641e-6</v>
       </c>
       <c r="C16">
-        <v>0.0027695881148090957</v>
+        <v>0.0027695881148090953</v>
       </c>
       <c r="D16">
-        <v>0.6067594896739704</v>
+        <v>0.6067594896739706</v>
       </c>
       <c r="E16">
         <v>0.0</v>
@@ -1079,25 +1079,25 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <v>1.7694087317880527e-6</v>
+        <v>1.7694087317880631e-6</v>
       </c>
       <c r="C17">
-        <v>0.0024823672984898137</v>
+        <v>0.0024823672984898154</v>
       </c>
       <c r="D17">
-        <v>0.8293355269571968</v>
+        <v>0.8293355269571969</v>
       </c>
       <c r="E17">
         <v>50.0</v>
       </c>
       <c r="F17">
-        <v>0.024418311007654847</v>
+        <v>0.02441831100765457</v>
       </c>
       <c r="G17">
-        <v>0.0008066469568351687</v>
+        <v>0.0008066469568351669</v>
       </c>
       <c r="H17">
-        <v>30.271373121468947</v>
+        <v>30.27137312146867</v>
       </c>
       <c r="I17">
         <v>4.76500000000002</v>
@@ -1114,25 +1114,25 @@
         <v>36</v>
       </c>
       <c r="B18">
-        <v>1.7022334651180513e-6</v>
+        <v>1.7022334651180585e-6</v>
       </c>
       <c r="C18">
-        <v>0.0012980796303208913</v>
+        <v>0.0012980796303208922</v>
       </c>
       <c r="D18">
-        <v>0.787351621328127</v>
+        <v>0.7873516213281273</v>
       </c>
       <c r="E18">
         <v>65.0</v>
       </c>
       <c r="F18">
-        <v>0.09103323966575691</v>
+        <v>0.0910332396657569</v>
       </c>
       <c r="G18">
-        <v>0.0020455270846322813</v>
+        <v>0.0020455270846322805</v>
       </c>
       <c r="H18">
-        <v>44.50356113574595</v>
+        <v>44.50356113574596</v>
       </c>
       <c r="I18">
         <v>5.87500000000001</v>
@@ -1149,10 +1149,10 @@
         <v>37</v>
       </c>
       <c r="B19">
-        <v>5.4466169182595184e-6</v>
+        <v>5.446616918259513e-6</v>
       </c>
       <c r="C19">
-        <v>0.002077195612999961</v>
+        <v>0.0020771956129999607</v>
       </c>
       <c r="D19">
         <v>0.9568215950859907</v>
@@ -1164,10 +1164,10 @@
         <v>0.005974111764135717</v>
       </c>
       <c r="G19">
-        <v>0.0008020929593548051</v>
+        <v>0.0008020929593548056</v>
       </c>
       <c r="H19">
-        <v>7.448153851071361</v>
+        <v>7.448153851071358</v>
       </c>
       <c r="I19">
         <v>8.97500000000002</v>
@@ -1184,25 +1184,25 @@
         <v>38</v>
       </c>
       <c r="B20">
-        <v>3.9191782655106795e-6</v>
+        <v>3.919178265510696e-6</v>
       </c>
       <c r="C20">
-        <v>0.0015086494781725384</v>
+        <v>0.0015086494781725408</v>
       </c>
       <c r="D20">
-        <v>0.9624609601056388</v>
+        <v>0.962460960105639</v>
       </c>
       <c r="E20">
         <v>105.0</v>
       </c>
       <c r="F20">
-        <v>0.12397395220127763</v>
+        <v>0.12397395220127744</v>
       </c>
       <c r="G20">
-        <v>0.0019001940164544992</v>
+        <v>0.0019001940164544969</v>
       </c>
       <c r="H20">
-        <v>65.24278633010117</v>
+        <v>65.24278633010114</v>
       </c>
       <c r="I20">
         <v>4.93500000000002</v>
@@ -1219,13 +1219,13 @@
         <v>39</v>
       </c>
       <c r="B21">
-        <v>3.2225057697024056e-6</v>
+        <v>3.2225057697024086e-6</v>
       </c>
       <c r="C21">
         <v>0.0022107474441920715</v>
       </c>
       <c r="D21">
-        <v>0.8691308888918737</v>
+        <v>0.8691308888918734</v>
       </c>
       <c r="E21">
         <v>10.0</v>
@@ -1254,25 +1254,25 @@
         <v>40</v>
       </c>
       <c r="B22">
-        <v>3.105379679947622e-6</v>
+        <v>3.105379679947639e-6</v>
       </c>
       <c r="C22">
-        <v>0.0026456023162226496</v>
+        <v>0.0026456023162226513</v>
       </c>
       <c r="D22">
-        <v>0.7315642281038814</v>
+        <v>0.7315642281038811</v>
       </c>
       <c r="E22">
         <v>30.0</v>
       </c>
       <c r="F22">
-        <v>0.0032854127164279323</v>
+        <v>0.0032854127164278907</v>
       </c>
       <c r="G22">
-        <v>0.0002864240236311365</v>
+        <v>0.0002864240236311348</v>
       </c>
       <c r="H22">
-        <v>11.470450958607309</v>
+        <v>11.470450958607232</v>
       </c>
       <c r="I22">
         <v>7.28500000000003</v>
@@ -1289,25 +1289,25 @@
         <v>41</v>
       </c>
       <c r="B23">
-        <v>6.342465855949505e-7</v>
+        <v>6.342465855949489e-7</v>
       </c>
       <c r="C23">
-        <v>0.0010118840668733955</v>
+        <v>0.0010118840668733953</v>
       </c>
       <c r="D23">
-        <v>0.31914427988310956</v>
+        <v>0.3191442798831098</v>
       </c>
       <c r="E23">
         <v>80.0</v>
       </c>
       <c r="F23">
-        <v>0.10688008411569574</v>
+        <v>0.1068800841156958</v>
       </c>
       <c r="G23">
-        <v>0.002116094528366658</v>
+        <v>0.0021160945283666584</v>
       </c>
       <c r="H23">
-        <v>50.508180368574024</v>
+        <v>50.508180368574045</v>
       </c>
       <c r="I23">
         <v>12.185</v>
@@ -1324,13 +1324,13 @@
         <v>42</v>
       </c>
       <c r="B24">
-        <v>1.901148553180244e-6</v>
+        <v>1.9011485531802405e-6</v>
       </c>
       <c r="C24">
-        <v>0.0027520218624565553</v>
+        <v>0.002752021862456555</v>
       </c>
       <c r="D24">
-        <v>0.5478121365925372</v>
+        <v>0.5478121365925368</v>
       </c>
       <c r="E24">
         <v>0.0</v>
@@ -1359,13 +1359,13 @@
         <v>43</v>
       </c>
       <c r="B25">
-        <v>1.527398125676187e-6</v>
+        <v>1.5273981256761882e-6</v>
       </c>
       <c r="C25">
-        <v>0.00023879107312494476</v>
+        <v>0.00023879107312494493</v>
       </c>
       <c r="D25">
-        <v>0.683988991419783</v>
+        <v>0.6839889914197832</v>
       </c>
       <c r="E25">
         <v>100.0</v>

</xml_diff>

<commit_message>
adding new data and new results
</commit_message>
<xml_diff>
--- a/data/exp_pro/integration_results.xlsx
+++ b/data/exp_pro/integration_results.xlsx
@@ -560,7 +560,7 @@
         <v>0.0028888213005892906</v>
       </c>
       <c r="D2">
-        <v>0.9837702690124214</v>
+        <v>0.9837702690124213</v>
       </c>
       <c r="E2">
         <v>0.0</v>
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>7.118242216056422e-6</v>
+        <v>7.118242216056418e-6</v>
       </c>
       <c r="C3">
         <v>0.0023564174254191994</v>
@@ -624,13 +624,13 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3.578991348692008e-6</v>
+        <v>3.578991348692013e-6</v>
       </c>
       <c r="C4">
-        <v>0.0030066570304212057</v>
+        <v>0.0030066570304212066</v>
       </c>
       <c r="D4">
-        <v>0.8537160291503734</v>
+        <v>0.8537160291503736</v>
       </c>
       <c r="E4">
         <v>0.0</v>
@@ -659,13 +659,13 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>4.256655561104181e-6</v>
+        <v>4.256655561104177e-6</v>
       </c>
       <c r="C5">
         <v>0.0030570173834040654</v>
       </c>
       <c r="D5">
-        <v>0.9133514435885822</v>
+        <v>0.9133514435885821</v>
       </c>
       <c r="E5">
         <v>0.0</v>
@@ -694,25 +694,25 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>3.4783850679157055e-6</v>
+        <v>3.478385067915703e-6</v>
       </c>
       <c r="C6">
-        <v>0.0018783308225360635</v>
+        <v>0.001878330822536063</v>
       </c>
       <c r="D6">
-        <v>0.8896796967247942</v>
+        <v>0.8896796967247943</v>
       </c>
       <c r="E6">
         <v>65.0</v>
       </c>
       <c r="F6">
-        <v>0.030665372006261377</v>
+        <v>0.03066537200626146</v>
       </c>
       <c r="G6">
-        <v>0.0011328828073544773</v>
+        <v>0.0011328828073544777</v>
       </c>
       <c r="H6">
-        <v>27.06844150797164</v>
+        <v>27.068441507971706</v>
       </c>
       <c r="I6">
         <v>3.0</v>
@@ -729,13 +729,13 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>4.091694782436062e-6</v>
+        <v>4.091694782436054e-6</v>
       </c>
       <c r="C7">
-        <v>0.0016430538673954237</v>
+        <v>0.0016430538673954224</v>
       </c>
       <c r="D7">
-        <v>0.9323074209011878</v>
+        <v>0.932307420901188</v>
       </c>
       <c r="E7">
         <v>65.0</v>
@@ -744,10 +744,10 @@
         <v>0.05978778447761897</v>
       </c>
       <c r="G7">
-        <v>0.0013449357914863747</v>
+        <v>0.001344935791486376</v>
       </c>
       <c r="H7">
-        <v>44.45400654520738</v>
+        <v>44.454006545207335</v>
       </c>
       <c r="I7">
         <v>5.56500000000003</v>
@@ -764,10 +764,10 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>2.982772219194521e-6</v>
+        <v>2.9827722191945188e-6</v>
       </c>
       <c r="C8">
-        <v>0.0005430912093717706</v>
+        <v>0.0005430912093717703</v>
       </c>
       <c r="D8">
         <v>0.8949963838513406</v>
@@ -776,13 +776,13 @@
         <v>10.0</v>
       </c>
       <c r="F8">
-        <v>0.0034499220167717136</v>
+        <v>0.003449922016771724</v>
       </c>
       <c r="G8">
-        <v>0.0006453632514853551</v>
+        <v>0.0006453632514853554</v>
       </c>
       <c r="H8">
-        <v>5.345705707338374</v>
+        <v>5.3457057073383885</v>
       </c>
       <c r="I8">
         <v>17.325</v>
@@ -799,22 +799,22 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <v>5.0196619977695655e-6</v>
+        <v>5.019661997769568e-6</v>
       </c>
       <c r="C9">
-        <v>0.0006868574715319699</v>
+        <v>0.0006868574715319702</v>
       </c>
       <c r="D9">
-        <v>0.7207989136707009</v>
+        <v>0.720798913670701</v>
       </c>
       <c r="E9">
         <v>20.0</v>
       </c>
       <c r="F9">
-        <v>0.02194280473629069</v>
+        <v>0.021942804736290688</v>
       </c>
       <c r="G9">
-        <v>0.0025378876695778462</v>
+        <v>0.002537887669577846</v>
       </c>
       <c r="H9">
         <v>8.646089816867534</v>
@@ -834,25 +834,25 @@
         <v>26</v>
       </c>
       <c r="B10">
-        <v>1.797695820229746e-6</v>
+        <v>1.797695820229706e-6</v>
       </c>
       <c r="C10">
-        <v>0.002217974601471791</v>
+        <v>0.002217974601471786</v>
       </c>
       <c r="D10">
-        <v>0.5815823553007161</v>
+        <v>0.5815823553007151</v>
       </c>
       <c r="E10">
         <v>50.0</v>
       </c>
       <c r="F10">
-        <v>0.02333094188092394</v>
+        <v>0.023330941880924133</v>
       </c>
       <c r="G10">
-        <v>0.0009650802861258024</v>
+        <v>0.0009650802861258072</v>
       </c>
       <c r="H10">
-        <v>24.17513052160994</v>
+        <v>24.175130521610022</v>
       </c>
       <c r="I10">
         <v>13.135</v>
@@ -869,13 +869,13 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <v>2.8192432208924357e-6</v>
+        <v>2.8192432208924366e-6</v>
       </c>
       <c r="C11">
         <v>0.0009498658740996753</v>
       </c>
       <c r="D11">
-        <v>0.933339618900605</v>
+        <v>0.9333396189006049</v>
       </c>
       <c r="E11">
         <v>30.0</v>
@@ -904,13 +904,13 @@
         <v>28</v>
       </c>
       <c r="B12">
-        <v>2.67810600981003e-6</v>
+        <v>2.6781060098100353e-6</v>
       </c>
       <c r="C12">
-        <v>0.002402806525398934</v>
+        <v>0.0024028065253989344</v>
       </c>
       <c r="D12">
-        <v>0.7326428057786221</v>
+        <v>0.732642805778622</v>
       </c>
       <c r="E12">
         <v>0.0</v>
@@ -939,13 +939,13 @@
         <v>29</v>
       </c>
       <c r="B13">
-        <v>4.4899438487943405e-6</v>
+        <v>4.48994384879435e-6</v>
       </c>
       <c r="C13">
-        <v>0.0030498559200348454</v>
+        <v>0.003049855920034846</v>
       </c>
       <c r="D13">
-        <v>0.7790251813239406</v>
+        <v>0.7790251813239407</v>
       </c>
       <c r="E13">
         <v>0.0</v>
@@ -980,7 +980,7 @@
         <v>0.002235039336088827</v>
       </c>
       <c r="D14">
-        <v>0.8725628538092224</v>
+        <v>0.8725628538092223</v>
       </c>
       <c r="E14">
         <v>30.0</v>
@@ -1009,25 +1009,25 @@
         <v>32</v>
       </c>
       <c r="B15">
-        <v>4.277303779273037e-6</v>
+        <v>4.277303779273057e-6</v>
       </c>
       <c r="C15">
-        <v>0.0023812930023717226</v>
+        <v>0.0023812930023717253</v>
       </c>
       <c r="D15">
-        <v>0.7424761480330686</v>
+        <v>0.7424761480330688</v>
       </c>
       <c r="E15">
         <v>65.0</v>
       </c>
       <c r="F15">
-        <v>0.03259641789730591</v>
+        <v>0.032596417897305746</v>
       </c>
       <c r="G15">
-        <v>0.0007214456521539678</v>
+        <v>0.0007214456521539652</v>
       </c>
       <c r="H15">
-        <v>45.18208377857037</v>
+        <v>45.18208377857031</v>
       </c>
       <c r="I15">
         <v>3.55500000000002</v>
@@ -1044,13 +1044,13 @@
         <v>33</v>
       </c>
       <c r="B16">
-        <v>3.754535179762641e-6</v>
+        <v>3.7545351797626435e-6</v>
       </c>
       <c r="C16">
-        <v>0.0027695881148090953</v>
+        <v>0.0027695881148090957</v>
       </c>
       <c r="D16">
-        <v>0.6067594896739706</v>
+        <v>0.6067594896739704</v>
       </c>
       <c r="E16">
         <v>0.0</v>
@@ -1079,25 +1079,25 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <v>1.7694087317880631e-6</v>
+        <v>1.7694087317880527e-6</v>
       </c>
       <c r="C17">
-        <v>0.0024823672984898154</v>
+        <v>0.0024823672984898137</v>
       </c>
       <c r="D17">
-        <v>0.8293355269571969</v>
+        <v>0.8293355269571968</v>
       </c>
       <c r="E17">
         <v>50.0</v>
       </c>
       <c r="F17">
-        <v>0.02441831100765457</v>
+        <v>0.024418311007654847</v>
       </c>
       <c r="G17">
-        <v>0.0008066469568351669</v>
+        <v>0.0008066469568351687</v>
       </c>
       <c r="H17">
-        <v>30.27137312146867</v>
+        <v>30.271373121468947</v>
       </c>
       <c r="I17">
         <v>4.76500000000002</v>
@@ -1114,25 +1114,25 @@
         <v>36</v>
       </c>
       <c r="B18">
-        <v>1.7022334651180585e-6</v>
+        <v>1.7022334651180513e-6</v>
       </c>
       <c r="C18">
-        <v>0.0012980796303208922</v>
+        <v>0.0012980796303208913</v>
       </c>
       <c r="D18">
-        <v>0.7873516213281273</v>
+        <v>0.787351621328127</v>
       </c>
       <c r="E18">
         <v>65.0</v>
       </c>
       <c r="F18">
-        <v>0.0910332396657569</v>
+        <v>0.09103323966575691</v>
       </c>
       <c r="G18">
-        <v>0.0020455270846322805</v>
+        <v>0.0020455270846322813</v>
       </c>
       <c r="H18">
-        <v>44.50356113574596</v>
+        <v>44.50356113574595</v>
       </c>
       <c r="I18">
         <v>5.87500000000001</v>
@@ -1149,10 +1149,10 @@
         <v>37</v>
       </c>
       <c r="B19">
-        <v>5.446616918259513e-6</v>
+        <v>5.4466169182595184e-6</v>
       </c>
       <c r="C19">
-        <v>0.0020771956129999607</v>
+        <v>0.002077195612999961</v>
       </c>
       <c r="D19">
         <v>0.9568215950859907</v>
@@ -1164,10 +1164,10 @@
         <v>0.005974111764135717</v>
       </c>
       <c r="G19">
-        <v>0.0008020929593548056</v>
+        <v>0.0008020929593548051</v>
       </c>
       <c r="H19">
-        <v>7.448153851071358</v>
+        <v>7.448153851071361</v>
       </c>
       <c r="I19">
         <v>8.97500000000002</v>
@@ -1184,25 +1184,25 @@
         <v>38</v>
       </c>
       <c r="B20">
-        <v>3.919178265510696e-6</v>
+        <v>3.9191782655106795e-6</v>
       </c>
       <c r="C20">
-        <v>0.0015086494781725408</v>
+        <v>0.0015086494781725384</v>
       </c>
       <c r="D20">
-        <v>0.962460960105639</v>
+        <v>0.9624609601056388</v>
       </c>
       <c r="E20">
         <v>105.0</v>
       </c>
       <c r="F20">
-        <v>0.12397395220127744</v>
+        <v>0.12397395220127763</v>
       </c>
       <c r="G20">
-        <v>0.0019001940164544969</v>
+        <v>0.0019001940164544992</v>
       </c>
       <c r="H20">
-        <v>65.24278633010114</v>
+        <v>65.24278633010117</v>
       </c>
       <c r="I20">
         <v>4.93500000000002</v>
@@ -1219,13 +1219,13 @@
         <v>39</v>
       </c>
       <c r="B21">
-        <v>3.2225057697024086e-6</v>
+        <v>3.2225057697024056e-6</v>
       </c>
       <c r="C21">
         <v>0.0022107474441920715</v>
       </c>
       <c r="D21">
-        <v>0.8691308888918734</v>
+        <v>0.8691308888918737</v>
       </c>
       <c r="E21">
         <v>10.0</v>
@@ -1254,25 +1254,25 @@
         <v>40</v>
       </c>
       <c r="B22">
-        <v>3.105379679947639e-6</v>
+        <v>3.105379679947622e-6</v>
       </c>
       <c r="C22">
-        <v>0.0026456023162226513</v>
+        <v>0.0026456023162226496</v>
       </c>
       <c r="D22">
-        <v>0.7315642281038811</v>
+        <v>0.7315642281038814</v>
       </c>
       <c r="E22">
         <v>30.0</v>
       </c>
       <c r="F22">
-        <v>0.0032854127164278907</v>
+        <v>0.0032854127164279323</v>
       </c>
       <c r="G22">
-        <v>0.0002864240236311348</v>
+        <v>0.0002864240236311365</v>
       </c>
       <c r="H22">
-        <v>11.470450958607232</v>
+        <v>11.470450958607309</v>
       </c>
       <c r="I22">
         <v>7.28500000000003</v>
@@ -1289,25 +1289,25 @@
         <v>41</v>
       </c>
       <c r="B23">
-        <v>6.342465855949489e-7</v>
+        <v>6.342465855949505e-7</v>
       </c>
       <c r="C23">
-        <v>0.0010118840668733953</v>
+        <v>0.0010118840668733955</v>
       </c>
       <c r="D23">
-        <v>0.3191442798831098</v>
+        <v>0.31914427988310956</v>
       </c>
       <c r="E23">
         <v>80.0</v>
       </c>
       <c r="F23">
-        <v>0.1068800841156958</v>
+        <v>0.10688008411569574</v>
       </c>
       <c r="G23">
-        <v>0.0021160945283666584</v>
+        <v>0.002116094528366658</v>
       </c>
       <c r="H23">
-        <v>50.508180368574045</v>
+        <v>50.508180368574024</v>
       </c>
       <c r="I23">
         <v>12.185</v>
@@ -1324,13 +1324,13 @@
         <v>42</v>
       </c>
       <c r="B24">
-        <v>1.9011485531802405e-6</v>
+        <v>1.901148553180244e-6</v>
       </c>
       <c r="C24">
-        <v>0.002752021862456555</v>
+        <v>0.0027520218624565553</v>
       </c>
       <c r="D24">
-        <v>0.5478121365925368</v>
+        <v>0.5478121365925372</v>
       </c>
       <c r="E24">
         <v>0.0</v>
@@ -1359,13 +1359,13 @@
         <v>43</v>
       </c>
       <c r="B25">
-        <v>1.5273981256761882e-6</v>
+        <v>1.527398125676187e-6</v>
       </c>
       <c r="C25">
-        <v>0.00023879107312494493</v>
+        <v>0.00023879107312494476</v>
       </c>
       <c r="D25">
-        <v>0.6839889914197832</v>
+        <v>0.683988991419783</v>
       </c>
       <c r="E25">
         <v>100.0</v>

</xml_diff>